<commit_message>
Restore important deleted files: faces, models, requirements.txt, and utility scripts
</commit_message>
<xml_diff>
--- a/attendance/attendance.xlsx
+++ b/attendance/attendance.xlsx
@@ -563,41 +563,15 @@
           <t>24BCY116-B</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2026-01-22 11:56:47</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>71.39</v>
-      </c>
-      <c r="G4" t="n">
-        <v>82.40026150430951</v>
-      </c>
-      <c r="H4" t="n">
-        <v>60.37714285714285</v>
-      </c>
-      <c r="I4" t="n">
-        <v>71.38870218072618</v>
-      </c>
-      <c r="J4" t="n">
-        <v>7</v>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>REAL</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>combined_multi_frame</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">

</xml_diff>